<commit_message>
Added counts back to Suisun data that did not correspond to any measured lengths, added more documentation, fixed more station locations
</commit_message>
<xml_diff>
--- a/data-raw/Suisun/Suisun comments.xlsx
+++ b/data-raw/Suisun/Suisun comments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbashevkin\Documents\LTMRdata\data-raw\Suisun\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A5DCB9-85A6-4851-8147-60CC397AEC60}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE9FBD8-9E77-4199-B0EE-7640AF0D90D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="-2604" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8580" yWindow="6075" windowWidth="29235" windowHeight="13545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Suisun comments" sheetId="1" r:id="rId1"/>
@@ -11632,8 +11632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O1189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G73" workbookViewId="0">
-      <selection activeCell="I88" sqref="I88"/>
+    <sheetView tabSelected="1" topLeftCell="A1172" workbookViewId="0">
+      <selection activeCell="I1187" sqref="I1187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50050,7 +50050,7 @@
         <v>69</v>
       </c>
       <c r="H1187">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I1187" s="3" t="s">
         <v>3553</v>

</xml_diff>